<commit_message>
CGE Calib Scenario defined + DMD_PRJ adj (dd files from previous commit)
dmd proj modified for ferroalloys
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B46A93-712B-4FDA-88B3-FA44A10DFE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09EC3DE-36AE-47AE-B563-8503B1B9B200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26610" windowHeight="13740" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="765" windowWidth="25890" windowHeight="15435" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="1096">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -3348,6 +3348,9 @@
   </si>
   <si>
     <t>Pdef-50</t>
+  </si>
+  <si>
+    <t>Pdef-55</t>
   </si>
 </sst>
 </file>
@@ -3945,13 +3948,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>468629</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -5954,42 +5957,42 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B3:K56"/>
+  <dimension ref="B3:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>6</v>
       </c>
@@ -5997,8 +6000,9 @@
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>23</v>
       </c>
@@ -6012,10 +6016,13 @@
         <v>1094</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>1095</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>1</v>
       </c>
@@ -6031,12 +6038,11 @@
       <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="H13">
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <f>B4</f>
-        <v>2017</v>
-      </c>
-      <c r="I13">
-        <f>$B$4</f>
         <v>2017</v>
       </c>
       <c r="J13">
@@ -6047,8 +6053,12 @@
         <f>$B$4</f>
         <v>2017</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f>$B$4</f>
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5">
         <v>1</v>
@@ -6062,24 +6072,27 @@
       <c r="F14" s="5">
         <v>1</v>
       </c>
-      <c r="H14">
-        <f>H13+F14</f>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f>I13+G14</f>
         <v>2018</v>
       </c>
-      <c r="I14">
-        <f>I13+C14</f>
+      <c r="J14">
+        <f>J13+C14</f>
         <v>2018</v>
       </c>
-      <c r="J14">
-        <f>J13+D14</f>
+      <c r="K14">
+        <f>K13+D14</f>
         <v>2018</v>
       </c>
-      <c r="K14">
-        <f>K13+E14</f>
+      <c r="L14">
+        <f>L13+E14</f>
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5">
         <v>1</v>
@@ -6093,24 +6106,27 @@
       <c r="F15" s="5">
         <v>1</v>
       </c>
-      <c r="H15">
-        <f t="shared" ref="H15:H56" si="0">H14+F15</f>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I56" si="0">I14+G15</f>
         <v>2019</v>
       </c>
-      <c r="I15">
-        <f t="shared" ref="I15:I27" si="1">I14+C15</f>
+      <c r="J15">
+        <f t="shared" ref="J15:J27" si="1">J14+C15</f>
         <v>2019</v>
       </c>
-      <c r="J15">
-        <f t="shared" ref="J15:K41" si="2">J14+D15</f>
+      <c r="K15">
+        <f>K14+D15</f>
         <v>2019</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
+      <c r="L15">
+        <f>L14+E15</f>
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5">
         <v>1</v>
@@ -6124,24 +6140,27 @@
       <c r="F16" s="5">
         <v>1</v>
       </c>
-      <c r="H16">
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="1"/>
         <v>2020</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
+      <c r="K16">
+        <f>K15+D16</f>
         <v>2020</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="2"/>
+      <c r="L16">
+        <f>L15+E16</f>
         <v>2020</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="5">
         <v>1</v>
@@ -6155,24 +6174,27 @@
       <c r="F17" s="5">
         <v>1</v>
       </c>
-      <c r="H17">
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="1"/>
         <v>2021</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
+      <c r="K17">
+        <f>K16+D17</f>
         <v>2021</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="2"/>
+      <c r="L17">
+        <f>L16+E17</f>
         <v>2021</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="5">
         <v>1</v>
@@ -6186,24 +6208,27 @@
       <c r="F18" s="5">
         <v>1</v>
       </c>
-      <c r="H18">
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
+      <c r="K18">
+        <f>K17+D18</f>
         <v>2022</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="2"/>
+      <c r="L18">
+        <f>L17+E18</f>
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="5">
         <v>1</v>
@@ -6217,24 +6242,27 @@
       <c r="F19" s="5">
         <v>1</v>
       </c>
-      <c r="H19">
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="1"/>
         <v>2023</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="2"/>
+      <c r="K19">
+        <f>K18+D19</f>
         <v>2023</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="2"/>
+      <c r="L19">
+        <f>L18+E19</f>
         <v>2023</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="5">
         <v>1</v>
@@ -6248,24 +6276,27 @@
       <c r="F20" s="5">
         <v>1</v>
       </c>
-      <c r="H20">
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="1"/>
         <v>2024</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
+      <c r="K20">
+        <f>K19+D20</f>
         <v>2024</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="2"/>
+      <c r="L20">
+        <f>L19+E20</f>
         <v>2024</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="5">
         <v>1</v>
@@ -6279,24 +6310,27 @@
       <c r="F21" s="5">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="1"/>
         <v>2025</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
+      <c r="K21">
+        <f>K20+D21</f>
         <v>2025</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="2"/>
+      <c r="L21">
+        <f>L20+E21</f>
         <v>2025</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="5">
         <v>1</v>
@@ -6310,24 +6344,27 @@
       <c r="F22" s="5">
         <v>1</v>
       </c>
-      <c r="H22">
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f t="shared" si="1"/>
         <v>2026</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
+      <c r="K22">
+        <f>K21+D22</f>
         <v>2026</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="2"/>
+      <c r="L22">
+        <f>L21+E22</f>
         <v>2026</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" s="5">
         <v>1</v>
@@ -6341,24 +6378,27 @@
       <c r="F23" s="5">
         <v>1</v>
       </c>
-      <c r="H23">
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="0"/>
         <v>2027</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="1"/>
         <v>2027</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
+      <c r="K23">
+        <f>K22+D23</f>
         <v>2027</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="2"/>
+      <c r="L23">
+        <f>L22+E23</f>
         <v>2027</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C24" s="5">
         <v>1</v>
       </c>
@@ -6371,24 +6411,27 @@
       <c r="F24" s="5">
         <v>1</v>
       </c>
-      <c r="H24">
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="1"/>
         <v>2028</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="2"/>
+      <c r="K24">
+        <f>K23+D24</f>
         <v>2028</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="2"/>
+      <c r="L24">
+        <f>L23+E24</f>
         <v>2028</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C25" s="5">
         <v>1</v>
       </c>
@@ -6401,24 +6444,27 @@
       <c r="F25" s="5">
         <v>1</v>
       </c>
-      <c r="H25">
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="1"/>
         <v>2029</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="2"/>
+      <c r="K25">
+        <f>K24+D25</f>
         <v>2029</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="2"/>
+      <c r="L25">
+        <f>L24+E25</f>
         <v>2029</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -6431,24 +6477,27 @@
       <c r="F26" s="5">
         <v>1</v>
       </c>
-      <c r="H26">
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f t="shared" si="1"/>
         <v>2030</v>
       </c>
-      <c r="J26">
-        <f t="shared" si="2"/>
+      <c r="K26">
+        <f>K25+D26</f>
         <v>2030</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="2"/>
+      <c r="L26">
+        <f>L25+E26</f>
         <v>2030</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C27" s="5"/>
       <c r="D27" s="5">
         <v>1</v>
@@ -6459,24 +6508,27 @@
       <c r="F27" s="5">
         <v>1</v>
       </c>
-      <c r="H27">
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="0"/>
         <v>2031</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="1"/>
         <v>2030</v>
       </c>
-      <c r="J27">
-        <f t="shared" si="2"/>
+      <c r="K27">
+        <f>K26+D27</f>
         <v>2031</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="2"/>
+      <c r="L27">
+        <f>L26+E27</f>
         <v>2031</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D28" s="5">
         <v>1</v>
       </c>
@@ -6486,20 +6538,23 @@
       <c r="F28" s="5">
         <v>1</v>
       </c>
-      <c r="H28">
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="2"/>
+      <c r="K28">
+        <f>K27+D28</f>
         <v>2032</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="2"/>
+      <c r="L28">
+        <f>L27+E28</f>
         <v>2032</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D29" s="5">
         <v>1</v>
       </c>
@@ -6509,20 +6564,23 @@
       <c r="F29" s="5">
         <v>1</v>
       </c>
-      <c r="H29">
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="0"/>
         <v>2033</v>
       </c>
-      <c r="J29">
-        <f t="shared" si="2"/>
+      <c r="K29">
+        <f>K28+D29</f>
         <v>2033</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="2"/>
+      <c r="L29">
+        <f>L28+E29</f>
         <v>2033</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D30" s="5">
         <v>1</v>
       </c>
@@ -6532,20 +6590,23 @@
       <c r="F30" s="5">
         <v>1</v>
       </c>
-      <c r="H30">
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="0"/>
         <v>2034</v>
       </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
+      <c r="K30">
+        <f>K29+D30</f>
         <v>2034</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="2"/>
+      <c r="L30">
+        <f>L29+E30</f>
         <v>2034</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D31" s="5">
         <v>1</v>
       </c>
@@ -6555,20 +6616,23 @@
       <c r="F31" s="5">
         <v>1</v>
       </c>
-      <c r="H31">
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="2"/>
+      <c r="K31">
+        <f>K30+D31</f>
         <v>2035</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="2"/>
+      <c r="L31">
+        <f>L30+E31</f>
         <v>2035</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D32" s="5">
         <v>1</v>
       </c>
@@ -6578,20 +6642,23 @@
       <c r="F32" s="5">
         <v>1</v>
       </c>
-      <c r="H32">
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="0"/>
         <v>2036</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="2"/>
+      <c r="K32">
+        <f>K31+D32</f>
         <v>2036</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="2"/>
+      <c r="L32">
+        <f>L31+E32</f>
         <v>2036</v>
       </c>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D33" s="5">
         <v>1</v>
       </c>
@@ -6601,20 +6668,23 @@
       <c r="F33" s="5">
         <v>1</v>
       </c>
-      <c r="H33">
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="0"/>
         <v>2037</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="2"/>
+      <c r="K33">
+        <f>K32+D33</f>
         <v>2037</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="2"/>
+      <c r="L33">
+        <f>L32+E33</f>
         <v>2037</v>
       </c>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D34" s="5">
         <v>1</v>
       </c>
@@ -6624,20 +6694,23 @@
       <c r="F34" s="5">
         <v>1</v>
       </c>
-      <c r="H34">
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="0"/>
         <v>2038</v>
       </c>
-      <c r="J34">
-        <f t="shared" si="2"/>
+      <c r="K34">
+        <f>K33+D34</f>
         <v>2038</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="2"/>
+      <c r="L34">
+        <f>L33+E34</f>
         <v>2038</v>
       </c>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D35" s="5">
         <v>1</v>
       </c>
@@ -6647,20 +6720,23 @@
       <c r="F35" s="5">
         <v>1</v>
       </c>
-      <c r="H35">
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="0"/>
         <v>2039</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="2"/>
+      <c r="K35">
+        <f>K34+D35</f>
         <v>2039</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="2"/>
+      <c r="L35">
+        <f>L34+E35</f>
         <v>2039</v>
       </c>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D36" s="5">
         <v>1</v>
       </c>
@@ -6670,283 +6746,331 @@
       <c r="F36" s="5">
         <v>1</v>
       </c>
-      <c r="H36">
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
-      <c r="J36">
-        <f t="shared" si="2"/>
+      <c r="K36">
+        <f>K35+D36</f>
         <v>2040</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="2"/>
+      <c r="L36">
+        <f>L35+E36</f>
         <v>2040</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E37" s="5">
         <v>1</v>
       </c>
       <c r="F37" s="5">
         <v>1</v>
       </c>
-      <c r="H37">
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="0"/>
         <v>2041</v>
       </c>
-      <c r="J37">
-        <f t="shared" si="2"/>
+      <c r="K37">
+        <f>K36+D37</f>
         <v>2040</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="2"/>
+      <c r="L37">
+        <f>L36+E37</f>
         <v>2041</v>
       </c>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E38" s="5">
         <v>1</v>
       </c>
       <c r="F38" s="5">
         <v>1</v>
       </c>
-      <c r="H38">
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="I38">
         <f t="shared" si="0"/>
         <v>2042</v>
       </c>
-      <c r="J38">
-        <f t="shared" si="2"/>
+      <c r="K38">
+        <f>K37+D38</f>
         <v>2040</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="2"/>
+      <c r="L38">
+        <f>L37+E38</f>
         <v>2042</v>
       </c>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E39" s="5">
         <v>1</v>
       </c>
       <c r="F39" s="5">
         <v>1</v>
       </c>
-      <c r="H39">
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <f t="shared" si="0"/>
         <v>2043</v>
       </c>
-      <c r="J39">
-        <f t="shared" si="2"/>
+      <c r="K39">
+        <f>K38+D39</f>
         <v>2040</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="2"/>
+      <c r="L39">
+        <f>L38+E39</f>
         <v>2043</v>
       </c>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E40" s="5">
         <v>1</v>
       </c>
       <c r="F40" s="5">
         <v>1</v>
       </c>
-      <c r="H40">
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
-      <c r="J40">
-        <f t="shared" si="2"/>
+      <c r="K40">
+        <f>K39+D40</f>
         <v>2040</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="2"/>
+      <c r="L40">
+        <f>L39+E40</f>
         <v>2044</v>
       </c>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E41" s="5">
         <v>1</v>
       </c>
       <c r="F41" s="5">
         <v>1</v>
       </c>
-      <c r="H41">
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
-      <c r="K41">
-        <f t="shared" si="2"/>
+      <c r="L41">
+        <f>L40+E41</f>
         <v>2045</v>
       </c>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E42" s="5">
         <v>1</v>
       </c>
       <c r="F42" s="5">
         <v>1</v>
       </c>
-      <c r="H42">
+      <c r="G42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="0"/>
         <v>2046</v>
       </c>
-      <c r="K42">
-        <f t="shared" ref="K42:K48" si="3">K41+E42</f>
+      <c r="L42">
+        <f t="shared" ref="L42:L48" si="2">L41+E42</f>
         <v>2046</v>
       </c>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E43" s="5">
         <v>1</v>
       </c>
       <c r="F43" s="5">
         <v>1</v>
       </c>
-      <c r="H43">
+      <c r="G43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="0"/>
         <v>2047</v>
       </c>
-      <c r="K43">
-        <f t="shared" si="3"/>
+      <c r="L43">
+        <f t="shared" si="2"/>
         <v>2047</v>
       </c>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E44" s="5">
         <v>1</v>
       </c>
       <c r="F44" s="5">
         <v>1</v>
       </c>
-      <c r="H44">
+      <c r="G44" s="5">
+        <v>1</v>
+      </c>
+      <c r="I44">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-      <c r="K44">
-        <f t="shared" si="3"/>
+      <c r="L44">
+        <f t="shared" si="2"/>
         <v>2048</v>
       </c>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E45" s="5">
         <v>1</v>
       </c>
       <c r="F45" s="5">
         <v>1</v>
       </c>
-      <c r="H45">
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45">
         <f t="shared" si="0"/>
         <v>2049</v>
       </c>
-      <c r="K45">
-        <f t="shared" si="3"/>
+      <c r="L45">
+        <f t="shared" si="2"/>
         <v>2049</v>
       </c>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E46" s="5">
         <v>1</v>
       </c>
       <c r="F46" s="5">
         <v>1</v>
       </c>
-      <c r="H46">
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46">
         <f t="shared" si="0"/>
         <v>2050</v>
       </c>
-      <c r="K46">
-        <f t="shared" si="3"/>
+      <c r="L46">
+        <f t="shared" si="2"/>
         <v>2050</v>
       </c>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.2">
       <c r="F47" s="5">
         <v>1</v>
       </c>
-      <c r="H47">
+      <c r="G47" s="5">
+        <v>1</v>
+      </c>
+      <c r="I47">
         <f t="shared" si="0"/>
         <v>2051</v>
       </c>
-      <c r="K47">
-        <f t="shared" si="3"/>
+      <c r="L47">
+        <f t="shared" si="2"/>
         <v>2050</v>
       </c>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.2">
       <c r="F48" s="5">
         <v>1</v>
       </c>
-      <c r="H48">
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
+      <c r="I48">
         <f t="shared" si="0"/>
         <v>2052</v>
       </c>
-      <c r="K48">
-        <f t="shared" si="3"/>
+      <c r="L48">
+        <f t="shared" si="2"/>
         <v>2050</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F49" s="5">
         <v>1</v>
       </c>
-      <c r="H49">
+      <c r="G49" s="5">
+        <v>1</v>
+      </c>
+      <c r="I49">
         <f t="shared" si="0"/>
         <v>2053</v>
       </c>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F50" s="5">
         <v>1</v>
       </c>
-      <c r="H50">
+      <c r="G50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <f t="shared" si="0"/>
         <v>2054</v>
       </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F51" s="5">
         <v>1</v>
       </c>
-      <c r="H51">
+      <c r="G51" s="5">
+        <v>1</v>
+      </c>
+      <c r="I51">
         <f t="shared" si="0"/>
         <v>2055</v>
       </c>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F52" s="5">
+    <row r="52" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G52" s="5">
         <v>5</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <f t="shared" si="0"/>
         <v>2060</v>
       </c>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F53" s="5">
+    <row r="53" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G53" s="5">
         <v>5</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <f t="shared" si="0"/>
         <v>2065</v>
       </c>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F54" s="5">
+    <row r="54" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G54" s="5">
         <v>5</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <f t="shared" si="0"/>
         <v>2070</v>
       </c>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="H55">
+    <row r="55" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I55">
         <f t="shared" si="0"/>
         <v>2070</v>
       </c>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="H56">
+    <row r="56" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I56">
         <f t="shared" si="0"/>
         <v>2070</v>
       </c>

</xml_diff>